<commit_message>
idiomaticize: use objects for target value storage
</commit_message>
<xml_diff>
--- a/RemoteYearBot/SampleData_RealAnon2020/fromBot_StudentSchedules.xlsx
+++ b/RemoteYearBot/SampleData_RealAnon2020/fromBot_StudentSchedules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="94">
   <si>
     <t>Chekov, Pavel</t>
   </si>
@@ -190,31 +190,112 @@
     <t>Friday, Feb 12th, 3:30-4:00</t>
   </si>
   <si>
+    <t>James Brody</t>
+  </si>
+  <si>
+    <t>Jose Ranz</t>
+  </si>
+  <si>
     <t>...</t>
   </si>
   <si>
+    <t>Maksim Plikus</t>
+  </si>
+  <si>
+    <t>Eric Potma</t>
+  </si>
+  <si>
+    <t>Celia Faiola</t>
+  </si>
+  <si>
+    <t>Vivek Swarup</t>
+  </si>
+  <si>
+    <t>Dae Seok Eom</t>
+  </si>
+  <si>
+    <t>Clare Yu</t>
+  </si>
+  <si>
+    <t>Wayne Hayes</t>
+  </si>
+  <si>
+    <t>John Lowengrub</t>
+  </si>
+  <si>
+    <t>Thomas Schilling</t>
+  </si>
+  <si>
+    <t>Grace Yuh Chwen Lee</t>
+  </si>
+  <si>
+    <t>Armando Villalta</t>
+  </si>
+  <si>
     <t>Kevin Thornton</t>
   </si>
   <si>
     <t>Jun Allard</t>
   </si>
   <si>
-    <t>John Lowengrub</t>
-  </si>
-  <si>
-    <t>Albert Siryaporn</t>
+    <t>Steven Allison</t>
+  </si>
+  <si>
+    <t>Dominik Wodarz</t>
+  </si>
+  <si>
+    <t>Kevin Beier</t>
   </si>
   <si>
     <t>Kyoko Yokomori</t>
   </si>
   <si>
-    <t>Dae Seok Eom</t>
-  </si>
-  <si>
-    <t>Vivek Swarup</t>
-  </si>
-  <si>
-    <t>Dominik Wodarz</t>
+    <t>Marcus Seldin</t>
+  </si>
+  <si>
+    <t>Arthur Lander</t>
+  </si>
+  <si>
+    <t>Jin Yu</t>
+  </si>
+  <si>
+    <t>Chang Liu</t>
+  </si>
+  <si>
+    <t>Ali Mortazavi</t>
+  </si>
+  <si>
+    <t>Knut Solna</t>
+  </si>
+  <si>
+    <t>Steve Frank</t>
+  </si>
+  <si>
+    <t>Alejandra Verdugo</t>
+  </si>
+  <si>
+    <t>Jack Xin</t>
+  </si>
+  <si>
+    <t>Ilhem Messaoudi</t>
+  </si>
+  <si>
+    <t>Anya Grosberg</t>
+  </si>
+  <si>
+    <t>Zeba Wunderlich</t>
+  </si>
+  <si>
+    <t>Reginald McNulty</t>
+  </si>
+  <si>
+    <t>Matt McHenry</t>
+  </si>
+  <si>
+    <t>Tim Downing</t>
+  </si>
+  <si>
+    <t>Katrine Whiteson</t>
   </si>
 </sst>
 </file>
@@ -666,79 +747,79 @@
         <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -746,82 +827,82 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N3" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="O3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q3" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="R3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T3" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="U3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -829,82 +910,82 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V4" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="W4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -912,82 +993,82 @@
         <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M5" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="N5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T5" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="U5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -995,82 +1076,82 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="S6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -1078,82 +1159,82 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -1161,82 +1242,82 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
         <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L8" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="M8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O8" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="P8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1244,82 +1325,82 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K9" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="L9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P9" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="Q9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -1327,82 +1408,82 @@
         <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
         <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="L10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O10" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="P10" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="Q10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S10" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="T10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U10" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="V10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y10" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="Z10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -1410,82 +1491,82 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W11" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="X11" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="Y11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -1493,82 +1574,82 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="L12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -1576,82 +1657,82 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L13" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="N13" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="O13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="R13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S13" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="T13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -1659,82 +1740,82 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V14" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="W14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:27">
@@ -1742,82 +1823,82 @@
         <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="I15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -1825,82 +1906,82 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V16" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="W16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -1908,82 +1989,82 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V17" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="W17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X17" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="Y17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -1991,82 +2072,82 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I18" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="J18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T18" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="U18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X18" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="Y18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -2074,82 +2155,82 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O19" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="P19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -2157,82 +2238,82 @@
         <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M20" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="N20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R20" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="S20" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="T20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z20" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="AA20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -2240,82 +2321,82 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="K21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T21" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="U21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V21" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="W21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z21" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="AA21" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -2323,82 +2404,82 @@
         <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P22" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="Q22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X22" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="Y22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -2406,82 +2487,82 @@
         <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="H23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U23" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="V23" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="W23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:27">
@@ -2489,82 +2570,82 @@
         <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L24" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="M24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V24" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="W24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y24" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="Z24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -2572,82 +2653,82 @@
         <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V25" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="W25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X25" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="Y25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -2655,82 +2736,82 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I26" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="J26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K26" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="L26" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="M26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:27">
@@ -2738,82 +2819,82 @@
         <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P27" t="s">
         <v>58</v>
       </c>
       <c r="Q27" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="R27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T27" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="U27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -2821,82 +2902,82 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G28" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="H28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J28" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="K28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:27">
@@ -2904,82 +2985,82 @@
         <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z29" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="AA29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -2987,82 +3068,82 @@
         <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H30" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="I30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L30" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="M30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P30" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="Q30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -3070,82 +3151,82 @@
         <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O31" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="P31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -3153,82 +3234,82 @@
         <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R32" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="S32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U32" t="s">
         <v>58</v>
       </c>
       <c r="V32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X32" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="Y32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Z32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA32" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:27">
@@ -3236,82 +3317,82 @@
         <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="T33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U33" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="V33" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="W33" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="X33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y33" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="Z33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved comments on module
</commit_message>
<xml_diff>
--- a/RemoteYearBot/SampleData_RealAnon2020/fromBot_StudentSchedules.xlsx
+++ b/RemoteYearBot/SampleData_RealAnon2020/fromBot_StudentSchedules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="97">
   <si>
     <t>Chekov, Pavel</t>
   </si>
@@ -196,121 +196,115 @@
     <t>Jin Yu</t>
   </si>
   <si>
+    <t>Clare Yu</t>
+  </si>
+  <si>
+    <t>Vivek Swarup</t>
+  </si>
+  <si>
+    <t>Jun Allard</t>
+  </si>
+  <si>
+    <t>Reginald McNulty</t>
+  </si>
+  <si>
+    <t>Alejandra Verdugo</t>
+  </si>
+  <si>
+    <t>Wayne Hayes</t>
+  </si>
+  <si>
+    <t>Scott Atwood</t>
+  </si>
+  <si>
+    <t>Armando Villalta</t>
+  </si>
+  <si>
+    <t>Thomas Schilling</t>
+  </si>
+  <si>
+    <t>Celia Faiola</t>
+  </si>
+  <si>
+    <t>Marcus Seldin</t>
+  </si>
+  <si>
+    <t>Ali Mortazavi</t>
+  </si>
+  <si>
+    <t>Chang Liu</t>
+  </si>
+  <si>
+    <t>Eric Potma</t>
+  </si>
+  <si>
+    <t>Dae Seok Eom</t>
+  </si>
+  <si>
+    <t>Kyoko Yokomori</t>
+  </si>
+  <si>
+    <t>James Brody</t>
+  </si>
+  <si>
+    <t>Katrine Whiteson</t>
+  </si>
+  <si>
+    <t>Matt McHenry</t>
+  </si>
+  <si>
     <t>Dominik Wodarz</t>
   </si>
   <si>
-    <t>Vivek Swarup</t>
-  </si>
-  <si>
-    <t>Matt McHenry</t>
+    <t>Kevin Thornton</t>
+  </si>
+  <si>
+    <t>Ilhem Messaoudi</t>
+  </si>
+  <si>
+    <t>Jose Ranz</t>
+  </si>
+  <si>
+    <t>John Lowengrub</t>
+  </si>
+  <si>
+    <t>Zeba Wunderlich</t>
+  </si>
+  <si>
+    <t>Qing Nie</t>
   </si>
   <si>
     <t>Maksim Plikus</t>
   </si>
   <si>
+    <t>Kevin Beier</t>
+  </si>
+  <si>
+    <t>Bruce Blumberg</t>
+  </si>
+  <si>
+    <t>Marian Waterman</t>
+  </si>
+  <si>
+    <t>Albert Siryaporn</t>
+  </si>
+  <si>
+    <t>Tim Downing</t>
+  </si>
+  <si>
+    <t>Arthur Lander</t>
+  </si>
+  <si>
+    <t>Steven Allison</t>
+  </si>
+  <si>
+    <t>Knut Solna</t>
+  </si>
+  <si>
+    <t>Steve Frank</t>
+  </si>
+  <si>
     <t>Anya Grosberg</t>
-  </si>
-  <si>
-    <t>Ali Mortazavi</t>
-  </si>
-  <si>
-    <t>Kyoko Yokomori</t>
-  </si>
-  <si>
-    <t>Chang Liu</t>
-  </si>
-  <si>
-    <t>Anne Calof</t>
-  </si>
-  <si>
-    <t>Katrine Whiteson</t>
-  </si>
-  <si>
-    <t>Thomas Schilling</t>
-  </si>
-  <si>
-    <t>Steve Frank</t>
-  </si>
-  <si>
-    <t>Kevin Thornton</t>
-  </si>
-  <si>
-    <t>Alejandra Verdugo</t>
-  </si>
-  <si>
-    <t>Jun Allard</t>
-  </si>
-  <si>
-    <t>James Brody</t>
-  </si>
-  <si>
-    <t>Ilhem Messaoudi</t>
-  </si>
-  <si>
-    <t>Marcus Seldin</t>
-  </si>
-  <si>
-    <t>Eric Potma</t>
-  </si>
-  <si>
-    <t>Armando Villalta</t>
-  </si>
-  <si>
-    <t>Dae Seok Eom</t>
-  </si>
-  <si>
-    <t>Wayne Hayes</t>
-  </si>
-  <si>
-    <t>Zeba Wunderlich</t>
-  </si>
-  <si>
-    <t>Scott Atwood</t>
-  </si>
-  <si>
-    <t>Steven Allison</t>
-  </si>
-  <si>
-    <t>Jose Ranz</t>
-  </si>
-  <si>
-    <t>John Lowengrub</t>
-  </si>
-  <si>
-    <t>Reginald McNulty</t>
-  </si>
-  <si>
-    <t>Qing Nie</t>
-  </si>
-  <si>
-    <t>Kevin Beier</t>
-  </si>
-  <si>
-    <t>Bruce Blumberg</t>
-  </si>
-  <si>
-    <t>Grace Yuh Chwen Lee</t>
-  </si>
-  <si>
-    <t>Clare Yu</t>
-  </si>
-  <si>
-    <t>Celia Faiola</t>
-  </si>
-  <si>
-    <t>Tim Downing</t>
-  </si>
-  <si>
-    <t>Marian Waterman</t>
-  </si>
-  <si>
-    <t>Jack Xin</t>
-  </si>
-  <si>
-    <t>Knut Solna</t>
-  </si>
-  <si>
-    <t>Albert Siryaporn</t>
   </si>
 </sst>
 </file>
@@ -777,10 +771,10 @@
         <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
         <v>58</v>
@@ -801,10 +795,10 @@
         <v>58</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="R2" t="s">
         <v>58</v>
@@ -860,10 +854,10 @@
         <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
         <v>58</v>
@@ -884,10 +878,10 @@
         <v>58</v>
       </c>
       <c r="P3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Q3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="R3" t="s">
         <v>58</v>
@@ -943,10 +937,10 @@
         <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J4" t="s">
         <v>58</v>
@@ -967,10 +961,10 @@
         <v>58</v>
       </c>
       <c r="P4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="Q4" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="R4" t="s">
         <v>58</v>
@@ -1026,11 +1020,11 @@
         <v>58</v>
       </c>
       <c r="H5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" t="s">
         <v>85</v>
       </c>
-      <c r="I5" t="s">
-        <v>81</v>
-      </c>
       <c r="J5" t="s">
         <v>58</v>
       </c>
@@ -1050,10 +1044,10 @@
         <v>58</v>
       </c>
       <c r="P5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Q5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="R5" t="s">
         <v>58</v>
@@ -1094,19 +1088,19 @@
         <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="H6" t="s">
         <v>58</v>
@@ -1139,19 +1133,19 @@
         <v>58</v>
       </c>
       <c r="R6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="S6" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="T6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="U6" t="s">
         <v>58</v>
       </c>
       <c r="V6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="W6" t="s">
         <v>58</v>
@@ -1163,10 +1157,10 @@
         <v>58</v>
       </c>
       <c r="Z6" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="AA6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -1177,79 +1171,79 @@
         <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" t="s">
+        <v>58</v>
+      </c>
+      <c r="P7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" t="s">
+        <v>59</v>
+      </c>
+      <c r="S7" t="s">
         <v>61</v>
       </c>
-      <c r="H7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" t="s">
-        <v>58</v>
-      </c>
-      <c r="L7" t="s">
-        <v>58</v>
-      </c>
-      <c r="M7" t="s">
-        <v>58</v>
-      </c>
-      <c r="N7" t="s">
-        <v>58</v>
-      </c>
-      <c r="O7" t="s">
-        <v>58</v>
-      </c>
-      <c r="P7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>58</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
+        <v>70</v>
+      </c>
+      <c r="U7" t="s">
+        <v>58</v>
+      </c>
+      <c r="V7" t="s">
+        <v>58</v>
+      </c>
+      <c r="W7" t="s">
+        <v>58</v>
+      </c>
+      <c r="X7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA7" t="s">
         <v>65</v>
-      </c>
-      <c r="S7" t="s">
-        <v>67</v>
-      </c>
-      <c r="T7" t="s">
-        <v>79</v>
-      </c>
-      <c r="U7" t="s">
-        <v>78</v>
-      </c>
-      <c r="V7" t="s">
-        <v>70</v>
-      </c>
-      <c r="W7" t="s">
-        <v>58</v>
-      </c>
-      <c r="X7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -1257,22 +1251,22 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="H8" t="s">
         <v>58</v>
@@ -1305,20 +1299,20 @@
         <v>58</v>
       </c>
       <c r="R8" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="S8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="T8" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="U8" t="s">
+        <v>86</v>
+      </c>
+      <c r="V8" t="s">
         <v>67</v>
       </c>
-      <c r="V8" t="s">
-        <v>64</v>
-      </c>
       <c r="W8" t="s">
         <v>58</v>
       </c>
@@ -1329,10 +1323,10 @@
         <v>58</v>
       </c>
       <c r="Z8" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="AA8" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1340,22 +1334,22 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H9" t="s">
         <v>58</v>
@@ -1388,19 +1382,19 @@
         <v>58</v>
       </c>
       <c r="R9" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="S9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="T9" t="s">
         <v>58</v>
       </c>
       <c r="U9" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="V9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="W9" t="s">
         <v>58</v>
@@ -1412,10 +1406,10 @@
         <v>58</v>
       </c>
       <c r="Z9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AA9" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -1447,13 +1441,13 @@
         <v>58</v>
       </c>
       <c r="J10" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="K10" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="L10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="M10" t="s">
         <v>58</v>
@@ -1486,13 +1480,13 @@
         <v>58</v>
       </c>
       <c r="W10" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="X10" t="s">
         <v>58</v>
       </c>
       <c r="Y10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Z10" t="s">
         <v>58</v>
@@ -1607,11 +1601,11 @@
         <v>58</v>
       </c>
       <c r="H12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" t="s">
         <v>86</v>
       </c>
-      <c r="I12" t="s">
-        <v>60</v>
-      </c>
       <c r="J12" t="s">
         <v>58</v>
       </c>
@@ -1631,10 +1625,10 @@
         <v>58</v>
       </c>
       <c r="P12" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="Q12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="R12" t="s">
         <v>58</v>
@@ -1690,11 +1684,11 @@
         <v>58</v>
       </c>
       <c r="H13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" t="s">
         <v>87</v>
       </c>
-      <c r="I13" t="s">
-        <v>63</v>
-      </c>
       <c r="J13" t="s">
         <v>58</v>
       </c>
@@ -1714,10 +1708,10 @@
         <v>58</v>
       </c>
       <c r="P13" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="Q13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="R13" t="s">
         <v>58</v>
@@ -1773,10 +1767,10 @@
         <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="J14" t="s">
         <v>58</v>
@@ -1797,10 +1791,10 @@
         <v>58</v>
       </c>
       <c r="P14" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="Q14" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="R14" t="s">
         <v>58</v>
@@ -1856,10 +1850,10 @@
         <v>58</v>
       </c>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J15" t="s">
         <v>58</v>
@@ -1880,10 +1874,10 @@
         <v>58</v>
       </c>
       <c r="P15" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="Q15" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="R15" t="s">
         <v>58</v>
@@ -1924,19 +1918,19 @@
         <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="F16" t="s">
         <v>58</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
         <v>58</v>
@@ -1969,34 +1963,34 @@
         <v>58</v>
       </c>
       <c r="R16" t="s">
+        <v>62</v>
+      </c>
+      <c r="S16" t="s">
+        <v>58</v>
+      </c>
+      <c r="T16" t="s">
+        <v>58</v>
+      </c>
+      <c r="U16" t="s">
+        <v>59</v>
+      </c>
+      <c r="V16" t="s">
+        <v>58</v>
+      </c>
+      <c r="W16" t="s">
+        <v>58</v>
+      </c>
+      <c r="X16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA16" t="s">
         <v>67</v>
-      </c>
-      <c r="S16" t="s">
-        <v>66</v>
-      </c>
-      <c r="T16" t="s">
-        <v>96</v>
-      </c>
-      <c r="U16" t="s">
-        <v>74</v>
-      </c>
-      <c r="V16" t="s">
-        <v>79</v>
-      </c>
-      <c r="W16" t="s">
-        <v>58</v>
-      </c>
-      <c r="X16" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -2007,19 +2001,19 @@
         <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F17" t="s">
         <v>58</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H17" t="s">
         <v>58</v>
@@ -2055,16 +2049,16 @@
         <v>58</v>
       </c>
       <c r="S17" t="s">
+        <v>58</v>
+      </c>
+      <c r="T17" t="s">
+        <v>67</v>
+      </c>
+      <c r="U17" t="s">
         <v>70</v>
       </c>
-      <c r="T17" t="s">
-        <v>58</v>
-      </c>
-      <c r="U17" t="s">
-        <v>59</v>
-      </c>
       <c r="V17" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="W17" t="s">
         <v>58</v>
@@ -2076,10 +2070,10 @@
         <v>58</v>
       </c>
       <c r="Z17" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="AA17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -2090,64 +2084,64 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" t="s">
+        <v>58</v>
+      </c>
+      <c r="N18" t="s">
+        <v>58</v>
+      </c>
+      <c r="O18" t="s">
+        <v>58</v>
+      </c>
+      <c r="P18" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>58</v>
+      </c>
+      <c r="R18" t="s">
+        <v>69</v>
+      </c>
+      <c r="S18" t="s">
+        <v>65</v>
+      </c>
+      <c r="T18" t="s">
         <v>75</v>
       </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" t="s">
-        <v>58</v>
-      </c>
-      <c r="I18" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K18" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" t="s">
-        <v>58</v>
-      </c>
-      <c r="M18" t="s">
-        <v>58</v>
-      </c>
-      <c r="N18" t="s">
-        <v>58</v>
-      </c>
-      <c r="O18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P18" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>58</v>
-      </c>
-      <c r="R18" t="s">
-        <v>76</v>
-      </c>
-      <c r="S18" t="s">
-        <v>86</v>
-      </c>
-      <c r="T18" t="s">
-        <v>64</v>
-      </c>
       <c r="U18" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="V18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W18" t="s">
         <v>58</v>
@@ -2159,10 +2153,10 @@
         <v>58</v>
       </c>
       <c r="Z18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="AA18" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -2173,65 +2167,65 @@
         <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
         <v>76</v>
       </c>
       <c r="E19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" t="s">
+        <v>58</v>
+      </c>
+      <c r="M19" t="s">
+        <v>58</v>
+      </c>
+      <c r="N19" t="s">
+        <v>58</v>
+      </c>
+      <c r="O19" t="s">
+        <v>58</v>
+      </c>
+      <c r="P19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>58</v>
+      </c>
+      <c r="R19" t="s">
+        <v>94</v>
+      </c>
+      <c r="S19" t="s">
+        <v>70</v>
+      </c>
+      <c r="T19" t="s">
+        <v>95</v>
+      </c>
+      <c r="U19" t="s">
+        <v>75</v>
+      </c>
+      <c r="V19" t="s">
         <v>80</v>
       </c>
-      <c r="F19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" t="s">
-        <v>83</v>
-      </c>
-      <c r="H19" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" t="s">
-        <v>58</v>
-      </c>
-      <c r="L19" t="s">
-        <v>58</v>
-      </c>
-      <c r="M19" t="s">
-        <v>58</v>
-      </c>
-      <c r="N19" t="s">
-        <v>58</v>
-      </c>
-      <c r="O19" t="s">
-        <v>58</v>
-      </c>
-      <c r="P19" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>58</v>
-      </c>
-      <c r="R19" t="s">
-        <v>77</v>
-      </c>
-      <c r="S19" t="s">
-        <v>69</v>
-      </c>
-      <c r="T19" t="s">
-        <v>86</v>
-      </c>
-      <c r="U19" t="s">
-        <v>87</v>
-      </c>
-      <c r="V19" t="s">
-        <v>60</v>
-      </c>
       <c r="W19" t="s">
         <v>58</v>
       </c>
@@ -2242,10 +2236,10 @@
         <v>58</v>
       </c>
       <c r="Z19" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="AA19" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -2277,52 +2271,52 @@
         <v>58</v>
       </c>
       <c r="J20" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="K20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20" t="s">
+        <v>58</v>
+      </c>
+      <c r="N20" t="s">
+        <v>83</v>
+      </c>
+      <c r="O20" t="s">
+        <v>58</v>
+      </c>
+      <c r="P20" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>58</v>
+      </c>
+      <c r="R20" t="s">
+        <v>58</v>
+      </c>
+      <c r="S20" t="s">
+        <v>58</v>
+      </c>
+      <c r="T20" t="s">
+        <v>58</v>
+      </c>
+      <c r="U20" t="s">
+        <v>58</v>
+      </c>
+      <c r="V20" t="s">
+        <v>58</v>
+      </c>
+      <c r="W20" t="s">
         <v>66</v>
       </c>
-      <c r="L20" t="s">
-        <v>64</v>
-      </c>
-      <c r="M20" t="s">
-        <v>58</v>
-      </c>
-      <c r="N20" t="s">
-        <v>79</v>
-      </c>
-      <c r="O20" t="s">
-        <v>58</v>
-      </c>
-      <c r="P20" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>58</v>
-      </c>
-      <c r="R20" t="s">
-        <v>58</v>
-      </c>
-      <c r="S20" t="s">
-        <v>58</v>
-      </c>
-      <c r="T20" t="s">
-        <v>58</v>
-      </c>
-      <c r="U20" t="s">
-        <v>58</v>
-      </c>
-      <c r="V20" t="s">
-        <v>58</v>
-      </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y20" t="s">
         <v>69</v>
-      </c>
-      <c r="X20" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>72</v>
       </c>
       <c r="Z20" t="s">
         <v>58</v>
@@ -2360,20 +2354,20 @@
         <v>58</v>
       </c>
       <c r="J21" t="s">
+        <v>79</v>
+      </c>
+      <c r="K21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" t="s">
+        <v>58</v>
+      </c>
+      <c r="N21" t="s">
         <v>60</v>
       </c>
-      <c r="K21" t="s">
-        <v>83</v>
-      </c>
-      <c r="L21" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" t="s">
-        <v>58</v>
-      </c>
-      <c r="N21" t="s">
-        <v>92</v>
-      </c>
       <c r="O21" t="s">
         <v>58</v>
       </c>
@@ -2399,13 +2393,13 @@
         <v>58</v>
       </c>
       <c r="W21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="X21" t="s">
         <v>58</v>
       </c>
       <c r="Y21" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="Z21" t="s">
         <v>58</v>
@@ -2452,13 +2446,13 @@
         <v>58</v>
       </c>
       <c r="M22" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="N22" t="s">
         <v>58</v>
       </c>
       <c r="O22" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="P22" t="s">
         <v>58</v>
@@ -2535,13 +2529,13 @@
         <v>58</v>
       </c>
       <c r="M23" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="N23" t="s">
         <v>58</v>
       </c>
       <c r="O23" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="P23" t="s">
         <v>58</v>
@@ -2568,7 +2562,7 @@
         <v>58</v>
       </c>
       <c r="X23" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="Y23" t="s">
         <v>58</v>
@@ -2618,13 +2612,13 @@
         <v>58</v>
       </c>
       <c r="M24" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="N24" t="s">
         <v>58</v>
       </c>
       <c r="O24" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="P24" t="s">
         <v>58</v>
@@ -2651,7 +2645,7 @@
         <v>58</v>
       </c>
       <c r="X24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Y24" t="s">
         <v>58</v>
@@ -2769,10 +2763,10 @@
         <v>58</v>
       </c>
       <c r="H26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I26" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="J26" t="s">
         <v>58</v>
@@ -2793,10 +2787,10 @@
         <v>58</v>
       </c>
       <c r="P26" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="Q26" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="R26" t="s">
         <v>58</v>
@@ -2852,10 +2846,10 @@
         <v>58</v>
       </c>
       <c r="H27" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="J27" t="s">
         <v>58</v>
@@ -2876,10 +2870,10 @@
         <v>58</v>
       </c>
       <c r="P27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q27" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="R27" t="s">
         <v>58</v>
@@ -2935,34 +2929,34 @@
         <v>58</v>
       </c>
       <c r="H28" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28" t="s">
+        <v>58</v>
+      </c>
+      <c r="K28" t="s">
+        <v>58</v>
+      </c>
+      <c r="L28" t="s">
+        <v>58</v>
+      </c>
+      <c r="M28" t="s">
+        <v>58</v>
+      </c>
+      <c r="N28" t="s">
+        <v>58</v>
+      </c>
+      <c r="O28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P28" t="s">
         <v>63</v>
       </c>
-      <c r="I28" t="s">
-        <v>78</v>
-      </c>
-      <c r="J28" t="s">
-        <v>58</v>
-      </c>
-      <c r="K28" t="s">
-        <v>58</v>
-      </c>
-      <c r="L28" t="s">
-        <v>58</v>
-      </c>
-      <c r="M28" t="s">
-        <v>58</v>
-      </c>
-      <c r="N28" t="s">
-        <v>58</v>
-      </c>
-      <c r="O28" t="s">
-        <v>58</v>
-      </c>
-      <c r="P28" t="s">
-        <v>74</v>
-      </c>
       <c r="Q28" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="R28" t="s">
         <v>58</v>
@@ -3018,10 +3012,10 @@
         <v>58</v>
       </c>
       <c r="H29" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="I29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J29" t="s">
         <v>58</v>
@@ -3042,10 +3036,10 @@
         <v>58</v>
       </c>
       <c r="P29" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q29" t="s">
         <v>88</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>82</v>
       </c>
       <c r="R29" t="s">
         <v>58</v>
@@ -3083,82 +3077,82 @@
         <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s">
         <v>77</v>
       </c>
       <c r="E30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" t="s">
+        <v>70</v>
+      </c>
+      <c r="H30" t="s">
+        <v>58</v>
+      </c>
+      <c r="I30" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" t="s">
+        <v>58</v>
+      </c>
+      <c r="K30" t="s">
+        <v>58</v>
+      </c>
+      <c r="L30" t="s">
+        <v>58</v>
+      </c>
+      <c r="M30" t="s">
+        <v>58</v>
+      </c>
+      <c r="N30" t="s">
+        <v>58</v>
+      </c>
+      <c r="O30" t="s">
+        <v>58</v>
+      </c>
+      <c r="P30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>58</v>
+      </c>
+      <c r="R30" t="s">
+        <v>58</v>
+      </c>
+      <c r="S30" t="s">
+        <v>58</v>
+      </c>
+      <c r="T30" t="s">
+        <v>58</v>
+      </c>
+      <c r="U30" t="s">
+        <v>73</v>
+      </c>
+      <c r="V30" t="s">
+        <v>58</v>
+      </c>
+      <c r="W30" t="s">
+        <v>58</v>
+      </c>
+      <c r="X30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA30" t="s">
         <v>59</v>
-      </c>
-      <c r="F30" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" t="s">
-        <v>74</v>
-      </c>
-      <c r="H30" t="s">
-        <v>58</v>
-      </c>
-      <c r="I30" t="s">
-        <v>58</v>
-      </c>
-      <c r="J30" t="s">
-        <v>58</v>
-      </c>
-      <c r="K30" t="s">
-        <v>58</v>
-      </c>
-      <c r="L30" t="s">
-        <v>58</v>
-      </c>
-      <c r="M30" t="s">
-        <v>58</v>
-      </c>
-      <c r="N30" t="s">
-        <v>58</v>
-      </c>
-      <c r="O30" t="s">
-        <v>58</v>
-      </c>
-      <c r="P30" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>58</v>
-      </c>
-      <c r="R30" t="s">
-        <v>96</v>
-      </c>
-      <c r="S30" t="s">
-        <v>81</v>
-      </c>
-      <c r="T30" t="s">
-        <v>73</v>
-      </c>
-      <c r="U30" t="s">
-        <v>58</v>
-      </c>
-      <c r="V30" t="s">
-        <v>61</v>
-      </c>
-      <c r="W30" t="s">
-        <v>58</v>
-      </c>
-      <c r="X30" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -3166,22 +3160,22 @@
         <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F31" t="s">
         <v>58</v>
       </c>
       <c r="G31" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H31" t="s">
         <v>58</v>
@@ -3214,19 +3208,19 @@
         <v>58</v>
       </c>
       <c r="R31" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="S31" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="T31" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="U31" t="s">
         <v>58</v>
       </c>
       <c r="V31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="W31" t="s">
         <v>58</v>
@@ -3241,7 +3235,7 @@
         <v>59</v>
       </c>
       <c r="AA31" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -3249,68 +3243,68 @@
         <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" t="s">
+        <v>58</v>
+      </c>
+      <c r="I32" t="s">
+        <v>58</v>
+      </c>
+      <c r="J32" t="s">
+        <v>58</v>
+      </c>
+      <c r="K32" t="s">
+        <v>58</v>
+      </c>
+      <c r="L32" t="s">
+        <v>58</v>
+      </c>
+      <c r="M32" t="s">
+        <v>58</v>
+      </c>
+      <c r="N32" t="s">
+        <v>58</v>
+      </c>
+      <c r="O32" t="s">
+        <v>58</v>
+      </c>
+      <c r="P32" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>58</v>
+      </c>
+      <c r="R32" t="s">
         <v>79</v>
       </c>
-      <c r="E32" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I32" t="s">
-        <v>58</v>
-      </c>
-      <c r="J32" t="s">
-        <v>58</v>
-      </c>
-      <c r="K32" t="s">
-        <v>58</v>
-      </c>
-      <c r="L32" t="s">
-        <v>58</v>
-      </c>
-      <c r="M32" t="s">
-        <v>58</v>
-      </c>
-      <c r="N32" t="s">
-        <v>58</v>
-      </c>
-      <c r="O32" t="s">
-        <v>58</v>
-      </c>
-      <c r="P32" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>58</v>
-      </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
+        <v>58</v>
+      </c>
+      <c r="T32" t="s">
+        <v>96</v>
+      </c>
+      <c r="U32" t="s">
+        <v>76</v>
+      </c>
+      <c r="V32" t="s">
         <v>83</v>
       </c>
-      <c r="S32" t="s">
-        <v>63</v>
-      </c>
-      <c r="T32" t="s">
-        <v>72</v>
-      </c>
-      <c r="U32" t="s">
-        <v>62</v>
-      </c>
-      <c r="V32" t="s">
-        <v>94</v>
-      </c>
       <c r="W32" t="s">
         <v>58</v>
       </c>
@@ -3321,10 +3315,10 @@
         <v>58</v>
       </c>
       <c r="Z32" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="AA32" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:27">

</xml_diff>